<commit_message>
todos los sp hechos, listos para probar
</commit_message>
<xml_diff>
--- a/ProyectoCheques/Repositorio/analisis.xlsx
+++ b/ProyectoCheques/Repositorio/analisis.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\DSC\DARWINET\darwincitoPrueba\ProyectoCheques\Repositorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Escritorio\programacion\DarwinGit\dsc-cursos\ProyectoCheques\Repositorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D8099F-74E3-48FD-B841-A0B0EC3712B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4815" windowHeight="5430"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TAREAS" sheetId="3" r:id="rId1"/>
@@ -645,7 +646,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -785,7 +786,13 @@
     <xdr:ext cx="4278923" cy="963081"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Imagen 9"/>
+        <xdr:cNvPr id="10" name="Imagen 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -823,7 +830,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Imagen 10"/>
+        <xdr:cNvPr id="11" name="Imagen 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -861,7 +874,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Imagen 12"/>
+        <xdr:cNvPr id="13" name="Imagen 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -899,7 +918,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Imagen 14"/>
+        <xdr:cNvPr id="15" name="Imagen 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -942,7 +967,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rectángulo 1"/>
+        <xdr:cNvPr id="2" name="Rectángulo 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1004,7 +1035,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Rectángulo 2"/>
+        <xdr:cNvPr id="3" name="Rectángulo 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1066,7 +1103,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Rectángulo 4"/>
+        <xdr:cNvPr id="5" name="Rectángulo 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1122,7 +1165,13 @@
     <xdr:ext cx="1843005" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="CuadroTexto 5"/>
+        <xdr:cNvPr id="6" name="CuadroTexto 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1178,7 +1227,13 @@
     <xdr:ext cx="1717430" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="CuadroTexto 6"/>
+        <xdr:cNvPr id="7" name="CuadroTexto 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1242,7 +1297,13 @@
     <xdr:ext cx="1359876" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="CuadroTexto 7"/>
+        <xdr:cNvPr id="8" name="CuadroTexto 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1306,7 +1367,13 @@
     <xdr:ext cx="1522534" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="CuadroTexto 8"/>
+        <xdr:cNvPr id="9" name="CuadroTexto 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1370,7 +1437,13 @@
     <xdr:ext cx="1909497" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="CuadroTexto 9"/>
+        <xdr:cNvPr id="10" name="CuadroTexto 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1426,7 +1499,13 @@
     <xdr:ext cx="1620187" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="CuadroTexto 10"/>
+        <xdr:cNvPr id="11" name="CuadroTexto 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1487,7 +1566,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="Rectángulo 11"/>
+        <xdr:cNvPr id="12" name="Rectángulo 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1556,7 +1641,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="Rectángulo 12"/>
+        <xdr:cNvPr id="13" name="Rectángulo 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1614,7 +1705,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="Rectángulo 14"/>
+        <xdr:cNvPr id="15" name="Rectángulo 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1665,7 +1762,13 @@
     <xdr:ext cx="1220912" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="CuadroTexto 15"/>
+        <xdr:cNvPr id="16" name="CuadroTexto 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1726,7 +1829,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="Rectángulo 16"/>
+        <xdr:cNvPr id="17" name="Rectángulo 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1795,7 +1904,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="Triángulo isósceles 17"/>
+        <xdr:cNvPr id="18" name="Triángulo isósceles 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000012000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1858,7 +1973,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="19" name="Rectángulo 18"/>
+        <xdr:cNvPr id="19" name="Rectángulo 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000013000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1935,7 +2056,13 @@
     <xdr:ext cx="1291507" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name="CuadroTexto 19"/>
+        <xdr:cNvPr id="20" name="CuadroTexto 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000014000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2018,7 +2145,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="Rectángulo 20"/>
+        <xdr:cNvPr id="21" name="Rectángulo 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000015000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2076,7 +2209,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="22" name="Rectángulo 21"/>
+        <xdr:cNvPr id="22" name="Rectángulo 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000016000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2146,7 +2285,13 @@
     <xdr:ext cx="2107756" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="23" name="CuadroTexto 22"/>
+        <xdr:cNvPr id="23" name="CuadroTexto 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000017000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2207,7 +2352,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="24" name="Rectángulo 23"/>
+        <xdr:cNvPr id="24" name="Rectángulo 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000018000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2276,7 +2427,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="25" name="Triángulo isósceles 24"/>
+        <xdr:cNvPr id="25" name="Triángulo isósceles 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000019000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2344,7 +2501,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rectángulo 1"/>
+        <xdr:cNvPr id="2" name="Rectángulo 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2406,7 +2569,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Rectángulo 2"/>
+        <xdr:cNvPr id="3" name="Rectángulo 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2463,7 +2632,13 @@
     <xdr:ext cx="1843005" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="CuadroTexto 4"/>
+        <xdr:cNvPr id="5" name="CuadroTexto 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2519,7 +2694,13 @@
     <xdr:ext cx="1717430" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="CuadroTexto 5"/>
+        <xdr:cNvPr id="6" name="CuadroTexto 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2583,7 +2764,13 @@
     <xdr:ext cx="1359876" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="CuadroTexto 6"/>
+        <xdr:cNvPr id="7" name="CuadroTexto 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2647,7 +2834,13 @@
     <xdr:ext cx="1522534" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="CuadroTexto 7"/>
+        <xdr:cNvPr id="8" name="CuadroTexto 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2711,7 +2904,13 @@
     <xdr:ext cx="566822" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="CuadroTexto 8"/>
+        <xdr:cNvPr id="9" name="CuadroTexto 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2772,7 +2971,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="Rectángulo 11"/>
+        <xdr:cNvPr id="12" name="Rectángulo 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2830,7 +3035,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="22" name="Rectángulo 21"/>
+        <xdr:cNvPr id="22" name="Rectángulo 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000016000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2894,7 +3105,13 @@
     <xdr:ext cx="581121" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="24" name="CuadroTexto 23"/>
+        <xdr:cNvPr id="24" name="CuadroTexto 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000018000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2955,7 +3172,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="25" name="Rectángulo 24"/>
+        <xdr:cNvPr id="25" name="Rectángulo 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000019000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3274,13 +3497,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="B3:F159"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3870,7 +4095,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:E19"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -3959,7 +4184,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="J3:K40"/>
   <sheetViews>
     <sheetView topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -4024,7 +4249,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="J3"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">

</xml_diff>

<commit_message>
creacion de reportes 1
</commit_message>
<xml_diff>
--- a/ProyectoCheques/Repositorio/analisis.xlsx
+++ b/ProyectoCheques/Repositorio/analisis.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Escritorio\programacion\DarwinGit\dsc-cursos\ProyectoCheques\Repositorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\DSC\DARWINET\darwincitoPrueba\ProyectoCheques\Repositorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D8099F-74E3-48FD-B841-A0B0EC3712B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TAREAS" sheetId="3" r:id="rId1"/>
     <sheet name="algoritmo" sheetId="2" r:id="rId2"/>
     <sheet name="GENERAR CHEQUES" sheetId="1" r:id="rId3"/>
     <sheet name="REPORTE GIROS" sheetId="4" r:id="rId4"/>
+    <sheet name="reportes" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="97">
   <si>
     <t>SE PUEDE INGRESAR POR LOTES</t>
   </si>
@@ -642,12 +642,18 @@
   <si>
     <t>hasta que numero de cheque filtramos los resultados del select</t>
   </si>
+  <si>
+    <t>3 COLUMNA</t>
+  </si>
+  <si>
+    <t>4 FILAS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -705,6 +711,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -738,7 +751,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -751,6 +764,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3235,6 +3249,543 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>366778</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>40864</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="342900" y="419100"/>
+          <a:ext cx="6119878" cy="3431764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectángulo 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="714375" y="809625"/>
+          <a:ext cx="5667375" cy="2686050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="00B0F0"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectángulo 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="733425" y="809625"/>
+          <a:ext cx="5667375" cy="895350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="00B0F0"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectángulo 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="733425" y="1704975"/>
+          <a:ext cx="5667375" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="00B0F0"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectángulo 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742950" y="1933575"/>
+          <a:ext cx="5667375" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="00B0F0"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectángulo 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="723900" y="2095499"/>
+          <a:ext cx="5667375" cy="276225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="00B0F0"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>695326</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectángulo 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="695326" y="514349"/>
+          <a:ext cx="2400300" cy="2962275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectángulo 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="704850" y="504824"/>
+          <a:ext cx="3905249" cy="2962275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectángulo 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="704850" y="504824"/>
+          <a:ext cx="5476875" cy="2962275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -3497,13 +4048,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="B3:F159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
@@ -4095,7 +4646,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E19"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -4184,10 +4735,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="J3:K40"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
@@ -4249,7 +4800,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="J3"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -4269,4 +4820,34 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="K4:K5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="11.42578125" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K4" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K5" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
darwin servicio city angular
</commit_message>
<xml_diff>
--- a/ProyectoCheques/Repositorio/analisis.xlsx
+++ b/ProyectoCheques/Repositorio/analisis.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\DSC\DARWINET\darwincitoPrueba\ProyectoCheques\Repositorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DARWIN\programacion\DarwinGit\dsc-cursos\ProyectoCheques\Repositorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386C2041-8443-4466-899D-9CD5F92D819D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TAREAS" sheetId="3" r:id="rId1"/>
@@ -17,6 +18,7 @@
     <sheet name="GENERAR CHEQUES" sheetId="1" r:id="rId3"/>
     <sheet name="REPORTE GIROS" sheetId="4" r:id="rId4"/>
     <sheet name="reportes" sheetId="5" r:id="rId5"/>
+    <sheet name="Hoja1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="103">
   <si>
     <t>SE PUEDE INGRESAR POR LOTES</t>
   </si>
@@ -648,11 +650,29 @@
   <si>
     <t>4 FILAS</t>
   </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>ANGULAR</t>
+  </si>
+  <si>
+    <t>creamos modelo response</t>
+  </si>
+  <si>
+    <t>para recibir la respuesta y guardarla en este modelo</t>
+  </si>
+  <si>
+    <t>creamos servicio</t>
+  </si>
+  <si>
+    <t>para pormedio de httpclient conectarnos al servicio y obtener la respuesta</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -719,7 +739,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -738,6 +758,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -751,7 +789,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -765,6 +803,9 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3266,7 +3307,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3310,7 +3357,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Rectángulo 2"/>
+        <xdr:cNvPr id="3" name="Rectángulo 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3371,7 +3424,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Rectángulo 3"/>
+        <xdr:cNvPr id="4" name="Rectángulo 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3432,7 +3491,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Rectángulo 4"/>
+        <xdr:cNvPr id="5" name="Rectángulo 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3493,7 +3558,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Rectángulo 5"/>
+        <xdr:cNvPr id="6" name="Rectángulo 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3554,7 +3625,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Rectángulo 7"/>
+        <xdr:cNvPr id="8" name="Rectángulo 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3615,7 +3692,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Rectángulo 8"/>
+        <xdr:cNvPr id="9" name="Rectángulo 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3676,7 +3759,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Rectángulo 9"/>
+        <xdr:cNvPr id="10" name="Rectángulo 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3737,7 +3826,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Rectángulo 10"/>
+        <xdr:cNvPr id="11" name="Rectángulo 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4048,7 +4143,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
@@ -4646,7 +4741,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:E19"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -4735,10 +4830,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="J3:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -4800,7 +4895,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="J3"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -4823,7 +4918,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="K4:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4850,4 +4945,94 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE7F5179-FAC1-403B-982F-1AFE55AEEBBF}">
+  <dimension ref="D1:K17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="9" width="11.42578125" style="13"/>
+    <col min="10" max="10" width="11.5703125" style="13" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="G1" s="14"/>
+    </row>
+    <row r="2" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="G2" s="14"/>
+    </row>
+    <row r="3" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D3" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="J3" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="G4" s="14"/>
+    </row>
+    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="G5" s="14"/>
+      <c r="J5" s="13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="G6" s="14"/>
+      <c r="K6" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="G7" s="14"/>
+      <c r="J7" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="G8" s="14"/>
+      <c r="K8" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="G13" s="14"/>
+    </row>
+    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="G14" s="14"/>
+    </row>
+    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="G15" s="14"/>
+    </row>
+    <row r="16" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
lista de ciudad completa
</commit_message>
<xml_diff>
--- a/ProyectoCheques/Repositorio/analisis.xlsx
+++ b/ProyectoCheques/Repositorio/analisis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DARWIN\programacion\DarwinGit\dsc-cursos\ProyectoCheques\Repositorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386C2041-8443-4466-899D-9CD5F92D819D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249C1F64-1C0C-4FB7-9C96-CB0082FABF99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="126">
   <si>
     <t>SE PUEDE INGRESAR POR LOTES</t>
   </si>
@@ -654,26 +654,255 @@
     <t>API</t>
   </si>
   <si>
-    <t>ANGULAR</t>
-  </si>
-  <si>
-    <t>creamos modelo response</t>
-  </si>
-  <si>
     <t>para recibir la respuesta y guardarla en este modelo</t>
   </si>
   <si>
-    <t>creamos servicio</t>
-  </si>
-  <si>
-    <t>para pormedio de httpclient conectarnos al servicio y obtener la respuesta</t>
+    <t>2 - creamos servicio</t>
+  </si>
+  <si>
+    <t>1 - creamos modelo response (interface)</t>
+  </si>
+  <si>
+    <t>para por medio de httpclient conectarnos al api y consumir un servicio</t>
+  </si>
+  <si>
+    <t>programa grande</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>f1 return "0915"</t>
+  </si>
+  <si>
+    <t>var x = f1</t>
+  </si>
+  <si>
+    <t>servicio</t>
+  </si>
+  <si>
+    <t>getCityAll (consumir servicio para obtener todas las ciudades en una variable observable)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">darwin se </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>suscribe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> a la promocion </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF66FFFF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dinosaurioObservable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF66FFFF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dinaosarioObservable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:  promocion </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>recibir  12  dinosaurios</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF66FFFF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cityObservable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:  promocion </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>recibir  todas las ciudades del ecuador</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">darwin se </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>suscribe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> a la promocion </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF66FFFF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cityObservable</t>
+    </r>
+  </si>
+  <si>
+    <t>APP</t>
+  </si>
+  <si>
+    <t>localhost:5170</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>localhost</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:4200</t>
+    </r>
+  </si>
+  <si>
+    <t>dominio del servidor</t>
+  </si>
+  <si>
+    <t>ip del sevidor</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>127.0.0.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:4200</t>
+    </r>
+  </si>
+  <si>
+    <t>127.0.0.1</t>
+  </si>
+  <si>
+    <t>19.168.100.5</t>
+  </si>
+  <si>
+    <t>0988876811</t>
+  </si>
+  <si>
+    <t>593-'0988876811</t>
+  </si>
+  <si>
+    <t>127.0.0.1:5170</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -738,6 +967,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -789,7 +1032,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -806,6 +1049,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3881,6 +4125,1060 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectángulo 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D5A6F79-7B7B-4A7F-8AA7-688FC2A87909}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2324100" y="9220200"/>
+          <a:ext cx="7505700" cy="2905125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-EC" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>152401</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>114301</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectángulo 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{286B5775-DF1C-4DEC-9E9D-9742E151F9A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3438526" y="8724900"/>
+          <a:ext cx="1485900" cy="866775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1600">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>192.168.0.5</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1600">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>127.0.0.1</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-EC" sz="1600">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>419101</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>371476</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectángulo 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8140552-5FEF-4676-955B-53FE8845EC15}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7515226" y="8848725"/>
+          <a:ext cx="1485900" cy="866775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1600">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>192.168.0.25</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1600">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>127.0.0.1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>95251</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectángulo 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33AED518-8671-4FA2-A755-3A4A015CBB70}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6429376" y="11630025"/>
+          <a:ext cx="1485900" cy="866775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B0F0"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1600">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>192.168.0.42</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1600">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>127.0.0.1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>439086</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>19147</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19DAFB40-EEBD-44D9-A13D-9D65CBF3ECD2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2362200" y="15897225"/>
+          <a:ext cx="6706536" cy="695422"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2466976" cy="969410"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="CuadroTexto 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{220441EA-F55C-4AE8-B62D-262AB0C87D9B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1590674" y="13992225"/>
+          <a:ext cx="2466976" cy="969410"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100"/>
+            <a:t>GetCityAll RETORNAR UN OBSERVABLE</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>538162</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>102635</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Conector recto de flecha 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98EC23AD-0A9E-4922-9DCD-B4228D2AFBF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="9" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2824162" y="14961635"/>
+          <a:ext cx="1471613" cy="983215"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1695450" cy="304801"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="CuadroTexto 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CAA55B4-BAE9-4D33-A3DC-E853CF51E794}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1657350" y="14316074"/>
+          <a:ext cx="1695450" cy="304801"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100"/>
+            <a:t>ICityGetAllResponse[]</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1752600" cy="647700"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="CuadroTexto 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10DAD500-F3B6-48D2-B11B-333249D90F02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1533526" y="17125950"/>
+          <a:ext cx="1752600" cy="647700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>METODO</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100"/>
+            <a:t> DEL SERVICIO</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100"/>
+            <a:t>GET</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>123826</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Conector recto de flecha 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{530C57B7-CC04-49E5-8020-1F258B172B8F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="15" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2409826" y="16249650"/>
+          <a:ext cx="1438274" cy="876300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1810624" cy="969410"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="CuadroTexto 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30F144F6-CE50-4237-A373-568042104189}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3648075" y="16964025"/>
+          <a:ext cx="1810624" cy="969410"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>RESPONSE</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100" baseline="0"/>
+            <a:t> DEL SERVICIO</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-EC" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>505262</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Conector recto de flecha 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E071183-0E7D-484D-922B-B5465465DE90}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="21" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4553387" y="16335375"/>
+          <a:ext cx="18613" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1695450" cy="304801"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="CuadroTexto 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE60D9D1-1A86-46FC-87AD-1491F5A07126}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3714750" y="17287874"/>
+          <a:ext cx="1695450" cy="304801"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100"/>
+            <a:t>ICityGetAllResponse</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>[]</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>752476</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1752600" cy="647700"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="CuadroTexto 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BE15E9B-0F65-477D-AFED-49D051DB1308}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6324601" y="17087850"/>
+          <a:ext cx="1752600" cy="647700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ENDPOINT</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100"/>
+            <a:t> DEL SERVICIO</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>104776</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Conector recto de flecha 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A888CA04-98CE-4B13-9923-2ADC3AA9E5E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="32" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="6705600" y="16325850"/>
+          <a:ext cx="495301" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Conector recto 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{790CC89F-A21E-4580-9C31-B22747381794}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3105150" y="16325850"/>
+          <a:ext cx="5895975" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -4833,7 +6131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="J3:K40"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -4921,8 +6219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="K4:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4949,90 +6247,181 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE7F5179-FAC1-403B-982F-1AFE55AEEBBF}">
-  <dimension ref="D1:K17"/>
+  <dimension ref="B1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="I76" sqref="I76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="11.42578125" style="13"/>
+    <col min="1" max="3" width="11.42578125" style="13"/>
+    <col min="4" max="4" width="15" style="13" customWidth="1"/>
+    <col min="5" max="9" width="11.42578125" style="13"/>
     <col min="10" max="10" width="11.5703125" style="13" customWidth="1"/>
     <col min="11" max="16384" width="11.42578125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="4:12" x14ac:dyDescent="0.25">
       <c r="G1" s="14"/>
-    </row>
-    <row r="2" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J1" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D2" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>125</v>
+      </c>
       <c r="G2" s="14"/>
-    </row>
-    <row r="3" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J2" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D3" s="15" t="s">
         <v>97</v>
       </c>
       <c r="G3" s="14"/>
       <c r="J3" s="15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="4:11" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="4:12" x14ac:dyDescent="0.25">
       <c r="G4" s="14"/>
     </row>
-    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:12" x14ac:dyDescent="0.25">
       <c r="G5" s="14"/>
       <c r="J5" s="13" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="4:12" x14ac:dyDescent="0.25">
       <c r="G6" s="14"/>
       <c r="K6" s="13" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="4:12" x14ac:dyDescent="0.25">
       <c r="G7" s="14"/>
       <c r="J7" s="13" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="4:11" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="4:12" x14ac:dyDescent="0.25">
       <c r="G8" s="14"/>
       <c r="K8" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G13" s="14"/>
+      <c r="J13" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="L13" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G14" s="14"/>
+      <c r="J14" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="L14" s="16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G15" s="14"/>
+    </row>
+    <row r="16" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="14"/>
+    </row>
+    <row r="24" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D24" s="13" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="G9" s="14"/>
-    </row>
-    <row r="10" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="G10" s="14"/>
-    </row>
-    <row r="11" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="G11" s="14"/>
-    </row>
-    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="G12" s="14"/>
-    </row>
-    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="G13" s="14"/>
-    </row>
-    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="G14" s="14"/>
-    </row>
-    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="G15" s="14"/>
-    </row>
-    <row r="16" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G17" s="14"/>
+    <row r="26" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D26" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D27" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="G28" s="13">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D34" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E35" s="13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>114</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsc: reporte date-range cheques
</commit_message>
<xml_diff>
--- a/ProyectoCheques/Repositorio/analisis.xlsx
+++ b/ProyectoCheques/Repositorio/analisis.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DARWIN\programacion\DarwinGit\dsc-cursos\ProyectoCheques\Repositorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\DSC\DARWINET\darwincitoPrueba\ProyectoCheques\Repositorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F6A084-E7B8-4201-8D0F-A3004CD706EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="TAREAS" sheetId="3" r:id="rId1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="171">
   <si>
     <t>SE PUEDE INGRESAR POR LOTES</t>
   </si>
@@ -1133,11 +1132,71 @@
       <t>: "papito"</t>
     </r>
   </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>BankName</t>
+  </si>
+  <si>
+    <t>AccountNumber</t>
+  </si>
+  <si>
+    <t>BeneficiaryName</t>
+  </si>
+  <si>
+    <t>ReportTypeName</t>
+  </si>
+  <si>
+    <t>CityName</t>
+  </si>
+  <si>
+    <t>ChequeNumber</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>PaymentDetail</t>
+  </si>
+  <si>
+    <t>Ecuatoriana de Comercio S.A.</t>
+  </si>
+  <si>
+    <t>Banco del Pacífico</t>
+  </si>
+  <si>
+    <t>DARWIN RODOLFO SANCHEZ CORREA</t>
+  </si>
+  <si>
+    <t>Reporte Individual</t>
+  </si>
+  <si>
+    <t> Amaluza</t>
+  </si>
+  <si>
+    <t>Detalle  general de cheques</t>
+  </si>
+  <si>
+    <t>NOMBRES Y APELLIDOS 1</t>
+  </si>
+  <si>
+    <t>NOMBRES Y APELLIDOS 2</t>
+  </si>
+  <si>
+    <t>NOMBRES Y APELLIDOS 3</t>
+  </si>
+  <si>
+    <t>NOMBRES Y APELLIDOS 4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1274,7 +1333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1294,6 +1353,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7231,7 +7291,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
@@ -7829,7 +7889,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E19"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -7918,7 +7978,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="J3:K40"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -7983,7 +8043,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="J3"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -8006,7 +8066,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="K4:K5"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -8036,7 +8096,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE7F5179-FAC1-403B-982F-1AFE55AEEBBF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L99"/>
   <sheetViews>
     <sheetView topLeftCell="A84" workbookViewId="0">
@@ -8218,7 +8278,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064DAA25-40A8-40A6-9A34-69A5977452C4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G26"/>
   <sheetViews>
     <sheetView topLeftCell="B33" workbookViewId="0">
@@ -8342,11 +8402,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B6E9CC2-F3DF-44C8-A092-7EA8CB272C9E}">
-  <dimension ref="C3:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8354,29 +8414,258 @@
     <col min="1" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="7" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <f>7*72</f>
+        <v>504</v>
+      </c>
+      <c r="C16" s="1">
+        <f>523/7</f>
+        <v>74.714285714285708</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <f>SUM(C19:L19)</f>
+        <v>504</v>
+      </c>
+      <c r="F19" s="1">
+        <v>110</v>
+      </c>
+      <c r="G19" s="1">
+        <v>70</v>
+      </c>
+      <c r="H19" s="1">
+        <v>70</v>
+      </c>
+      <c r="I19" s="1">
+        <v>30</v>
+      </c>
+      <c r="J19" s="1">
+        <v>40</v>
+      </c>
+      <c r="K19" s="1">
+        <v>40</v>
+      </c>
+      <c r="L19" s="1">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E21" s="1">
+        <v>11223344556677</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I21" s="1">
+        <v>1977</v>
+      </c>
+      <c r="J21" s="1">
+        <v>1453.33</v>
+      </c>
+      <c r="K21" s="19">
+        <v>45836</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E22" s="1">
+        <v>11223344556677</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I22" s="1">
+        <v>1978</v>
+      </c>
+      <c r="J22" s="1">
+        <v>123.34</v>
+      </c>
+      <c r="K22" s="19">
+        <v>45836</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C23" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E23" s="1">
+        <v>11223344556677</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I23" s="1">
+        <v>1979</v>
+      </c>
+      <c r="J23" s="1">
+        <v>223.34</v>
+      </c>
+      <c r="K23" s="19">
+        <v>45836</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C24" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E24" s="1">
+        <v>11223344556677</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I24" s="1">
+        <v>1980</v>
+      </c>
+      <c r="J24" s="1">
+        <v>323.33999999999997</v>
+      </c>
+      <c r="K24" s="19">
+        <v>45836</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C25" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E25" s="1">
+        <v>11223344556677</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I25" s="1">
+        <v>1981</v>
+      </c>
+      <c r="J25" s="1">
+        <v>423.34</v>
+      </c>
+      <c r="K25" s="19">
+        <v>45836</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>